<commit_message>
TS 1.7 New inputs raja 29/01/2022
</commit_message>
<xml_diff>
--- a/TS Jatai Working/TTD Krama PaaraayaNam-Kramam.xlsx
+++ b/TS Jatai Working/TTD Krama PaaraayaNam-Kramam.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24729"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0097E86C-A1A2-4639-9BBE-45C99B6AB161}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Kandam1 to 7" sheetId="1" r:id="rId1"/>
@@ -1111,7 +1112,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1664,6 +1665,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1699,6 +1717,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1874,11 +1909,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L207"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A197" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="F207" sqref="F207"/>
     </sheetView>
   </sheetViews>
@@ -5845,8 +5880,8 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="H24" r:id="rId1"/>
-    <hyperlink ref="H31" r:id="rId2"/>
+    <hyperlink ref="H24" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="H31" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId3"/>

</xml_diff>